<commit_message>
Ajout des colonnes aux matrices
</commit_message>
<xml_diff>
--- a/ressources/matrices/matrice_actifs.xlsx
+++ b/ressources/matrices/matrice_actifs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinlejeune/Desktop/TP_Audit_and_Sec_of_MedData/ressources/matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706E0CFA-E403-A043-A76B-23086B41FC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C876FEA0-D120-6D41-A4F2-8DA95F3613F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5000" yWindow="1220" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,22 +25,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>test2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Nature de l'équipement</t>
+  </si>
+  <si>
+    <t>Marque</t>
+  </si>
+  <si>
+    <t>Modèle</t>
+  </si>
+  <si>
+    <t>Type d'OS</t>
+  </si>
+  <si>
+    <t>Version OS</t>
+  </si>
+  <si>
+    <t>Hostname</t>
+  </si>
+  <si>
+    <t>Ports utilisés</t>
+  </si>
+  <si>
+    <t>Ports non utilisés/éteints/passifs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,17 +374,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>